<commit_message>
Update {mNIRS} functions and documentation
read_data.R: add function arguments for verbose, explicit sample_rate. replace_fixed_values.R: return NA by default, improve median at edges, simplify return vector. replace_missing_values.R: simplify return vector. replace_outliers.R: improve median at edges, simplify return vector. resample_dataframe.R: I think working binned downsampling for both `sample_column` = time and row_number. Need to verify
</commit_message>
<xml_diff>
--- a/inst/moxy_ramp_example.xlsx
+++ b/inst/moxy_ramp_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R-Projects\mNIRS\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39283E1-905F-4707-8FA6-001B0FE0335B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAA4CBC-7CE7-47D1-9703-9CC45FFCD784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4995" yWindow="1470" windowWidth="19410" windowHeight="28605" xr2:uid="{ED07EABD-9B2D-42C5-B904-3B14C8E7B28A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ED07EABD-9B2D-42C5-B904-3B14C8E7B28A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -7036,9 +7036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9183BCA-730E-4465-A692-010E8B3E5191}">
   <dimension ref="A1:D2204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A814" workbookViewId="0">
-      <selection activeCell="E872" sqref="E872"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>